<commit_message>
Actualización de la nueva dirección del Cronograma de implementación
</commit_message>
<xml_diff>
--- a/Documentos/ADM/PQRS_ADM_D_EsquemaAccesosSistemas.xlsx
+++ b/Documentos/ADM/PQRS_ADM_D_EsquemaAccesosSistemas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="120" windowWidth="11715" windowHeight="7485"/>
+    <workbookView xWindow="360" yWindow="120" windowWidth="11715" windowHeight="7485" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Repositorio Configuracion" sheetId="4" r:id="rId1"/>
@@ -73,15 +73,9 @@
     <t>Clave</t>
   </si>
   <si>
-    <t>https://www.tomsplanner.es/public/calendariodesarrollopqrs2</t>
-  </si>
-  <si>
     <t>Tom's Planner</t>
   </si>
   <si>
-    <t>calendario</t>
-  </si>
-  <si>
     <t>KanbanPad</t>
   </si>
   <si>
@@ -137,6 +131,12 @@
   </si>
   <si>
     <t>BitBucket</t>
+  </si>
+  <si>
+    <t>https://www.tomsplanner.es/public/calendariodesarrollo-pqrs2?</t>
+  </si>
+  <si>
+    <t>cronograma</t>
   </si>
 </sst>
 </file>
@@ -322,6 +322,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -330,24 +348,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -646,7 +646,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -660,20 +660,20 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1"/>
     <row r="2" spans="2:5" ht="16.5" thickBot="1">
-      <c r="B2" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="12"/>
+      <c r="B2" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" spans="2:5" ht="15.75" thickBot="1">
-      <c r="B3" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="7"/>
+      <c r="B3" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="13"/>
     </row>
     <row r="4" spans="2:5" ht="15.75" thickBot="1">
       <c r="B4" s="4"/>
@@ -682,59 +682,59 @@
       <c r="E4" s="3"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" thickBot="1">
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="15.75" thickBot="1">
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="15.75" thickBot="1">
+      <c r="B7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="15.75" thickBot="1">
+      <c r="B8" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" ht="15.75" thickBot="1">
-      <c r="B7" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="D8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" ht="15.75" thickBot="1">
-      <c r="B8" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -773,20 +773,20 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1"/>
     <row r="2" spans="2:5" ht="16.5" thickBot="1">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="12"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" spans="2:5" ht="15.75" thickBot="1">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="7"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="13"/>
     </row>
     <row r="4" spans="2:5" ht="15.75" thickBot="1">
       <c r="B4" s="4"/>
@@ -795,16 +795,16 @@
       <c r="E4" s="3"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" thickBot="1">
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="6" t="s">
         <v>17</v>
       </c>
     </row>
@@ -894,20 +894,20 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1"/>
     <row r="2" spans="2:5" ht="16.5" thickBot="1">
-      <c r="B2" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="12"/>
+      <c r="B2" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" spans="2:5" ht="15.75" thickBot="1">
-      <c r="B3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="7"/>
+      <c r="B3" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="13"/>
     </row>
     <row r="4" spans="2:5" ht="15.75" thickBot="1">
       <c r="B4" s="4"/>
@@ -916,59 +916,59 @@
       <c r="E4" s="3"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" thickBot="1">
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="15.75" thickBot="1">
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="15.75" thickBot="1">
+      <c r="B7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="15.75" thickBot="1">
+      <c r="B8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" ht="15.75" thickBot="1">
-      <c r="B7" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" ht="15.75" thickBot="1">
-      <c r="B8" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -993,8 +993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1007,20 +1007,20 @@
   <sheetData>
     <row r="1" spans="2:5" ht="15.75" thickBot="1"/>
     <row r="2" spans="2:5" ht="16.5" thickBot="1">
-      <c r="B2" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="12"/>
+      <c r="B2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" spans="2:5" ht="15.75" thickBot="1">
-      <c r="B3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="7"/>
+      <c r="B3" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="13"/>
     </row>
     <row r="4" spans="2:5" ht="15.75" thickBot="1">
       <c r="B4" s="4"/>
@@ -1029,16 +1029,16 @@
       <c r="E4" s="3"/>
     </row>
     <row r="5" spans="2:5" ht="15.75" thickBot="1">
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="6" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1047,7 +1047,7 @@
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>